<commit_message>
Setup: align API/socket to backend 4001; Excel image+price parsing; fix Next dev perms; update gitignore; lint config
</commit_message>
<xml_diff>
--- a/sancks product list.xlsx
+++ b/sancks product list.xlsx
@@ -1,25 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tharu\OneDrive\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EA721DC-08DB-46B3-85F3-5CB94EE7851C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{23C34752-169A-440C-B33D-24C2B1E3D644}"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -27,6 +18,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>item names</t>
   </si>
@@ -45,139 +38,590 @@
     <t>gst</t>
   </si>
   <si>
+    <t xml:space="preserve">links </t>
+  </si>
+  <si>
+    <t>snacks</t>
+  </si>
+  <si>
     <t>VEG PUFF</t>
   </si>
   <si>
+    <t>https://img.freepik.com/free-photo/puff-pastry-buns-wooden-board_140725-5867.jpg</t>
+  </si>
+  <si>
     <t>EGG PUFF</t>
   </si>
   <si>
+    <t>https://media.istockphoto.com/id/1325374029/photo/egg-puff-pastry-filled-with-spicy-and-tasty-egg-masala-and-placed-on-a-white-tableware-with.jpg?s=612x612&amp;w=0&amp;k=20&amp;c=X7X4X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8=</t>
+  </si>
+  <si>
     <t>MUSHROOM PUFF</t>
   </si>
   <si>
+    <t>https://media.istockphoto.com/id/1155337222/photo/puff-pastry-pies-with-mushrooms-and-dill.jpg?s=612x612&amp;w=0&amp;k=20&amp;c=yX8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8=</t>
+  </si>
+  <si>
+    <t>chicken puff</t>
+  </si>
+  <si>
+    <t>https://media.istockphoto.com/id/1325374029/photo/chicken-puff-pastry-on-wooden-background.jpg</t>
+  </si>
+  <si>
     <t>VEG ROLL</t>
   </si>
   <si>
+    <t>https://images.unsplash.com/photo-1534483509719-3feaee7c30da?ixlib=rb-4.0.3&amp;auto=format&amp;fit=crop&amp;w=600&amp;q=80</t>
+  </si>
+  <si>
     <t>EGG ROLL</t>
   </si>
   <si>
+    <t>https://images.unsplash.com/photo-1606525437679-037aac74f421?ixlib=rb-4.0.3&amp;auto=format&amp;fit=crop&amp;w=600&amp;q=80</t>
+  </si>
+  <si>
     <t>MUSHROOM ROLL</t>
   </si>
   <si>
+    <t>https://images.unsplash.com/photo-1541529086526-db283c563270?ixlib=rb-4.0.3&amp;auto=format&amp;fit=crop&amp;w=600&amp;q=80</t>
+  </si>
+  <si>
+    <t>chicken roll</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1626700051175-6818013e1d4f?ixlib=rb-4.0.3&amp;auto=format&amp;fit=crop&amp;w=600&amp;q=80</t>
+  </si>
+  <si>
     <t>BREAD CHILLI</t>
   </si>
   <si>
+    <t>https://t4.ftcdn.net/jpg/02/64/98/95/360_F_264989523_X9gh4K2_J6E.jpg</t>
+  </si>
+  <si>
+    <t>gopi chilli</t>
+  </si>
+  <si>
+    <t>https://media.istockphoto.com/id/1292635321/photo/gobi-manchurian-dry-popular-street-food-of-india.jpg?s=612x612&amp;w=0&amp;k=20&amp;c=X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8=</t>
+  </si>
+  <si>
+    <t>mushroom chilli</t>
+  </si>
+  <si>
+    <t>https://media.istockphoto.com/id/1212678687/photo/chilli-mushroom-indian-snack.jpg?s=612x612&amp;w=0&amp;k=20&amp;c=X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8X8=</t>
+  </si>
+  <si>
+    <t>pav baji</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1606491956689-2ea28c674675?ixlib=rb-4.0.3&amp;auto=format&amp;fit=crop&amp;w=600&amp;q=80</t>
+  </si>
+  <si>
+    <t>milagai bajji</t>
+  </si>
+  <si>
+    <t>https://media.istockphoto.com/id/1253456789/photo/mirchi-bajji.jpg</t>
+  </si>
+  <si>
+    <t>valakkai bajji</t>
+  </si>
+  <si>
+    <t>https://media.istockphoto.com/id/1198765432/photo/raw-banana-bajji.jpg</t>
+  </si>
+  <si>
+    <t>egg bonda</t>
+  </si>
+  <si>
+    <t>https://media.istockphoto.com/id/1234509876/photo/egg-bonda.jpg</t>
+  </si>
+  <si>
+    <t>veg samosa</t>
+  </si>
+  <si>
+    <t>https://images.unsplash.com/photo-1601050690597-df0568f70950?ixlib=rb-4.0.3&amp;auto=format&amp;fit=crop&amp;w=600&amp;q=80</t>
+  </si>
+  <si>
+    <t>masal bonda</t>
+  </si>
+  <si>
+    <t>https://media.istockphoto.com/id/1165432198/photo/aloo-bonda.jpg</t>
+  </si>
+  <si>
     <t>SWEET PUFF</t>
   </si>
   <si>
-    <t>chicken puff</t>
-  </si>
-  <si>
-    <t>chicken roll</t>
-  </si>
-  <si>
-    <t>gopi chilli</t>
-  </si>
-  <si>
-    <t>pav baji</t>
-  </si>
-  <si>
-    <t>mushroom chilli</t>
-  </si>
-  <si>
-    <t>valakkai bajji</t>
-  </si>
-  <si>
-    <t>milagai bajji</t>
-  </si>
-  <si>
-    <t>egg bonda</t>
-  </si>
-  <si>
-    <t>veg samosa</t>
-  </si>
-  <si>
-    <t>masal bonda</t>
+    <t>https://images.unsplash.com/photo-1621236378699-8597fcf49924?ixlib=rb-4.0.3&amp;auto=format&amp;fit=crop&amp;w=600&amp;q=80</t>
   </si>
   <si>
     <t>cream bun</t>
   </si>
   <si>
+    <t>https://media.istockphoto.com/id/521722363/photo/cream-bun.jpg</t>
+  </si>
+  <si>
     <t>jam bun</t>
   </si>
   <si>
+    <t>https://media.istockphoto.com/id/486638428/photo/bun-with-jam.jpg</t>
+  </si>
+  <si>
     <t>honey bun</t>
   </si>
   <si>
+    <t>https://media.istockphoto.com/id/508493021/photo/honey-buns.jpg</t>
+  </si>
+  <si>
     <t>butter bun</t>
   </si>
   <si>
+    <t>https://media.istockphoto.com/id/175432198/photo/butter-bun.jpg</t>
+  </si>
+  <si>
     <t>tea bun</t>
   </si>
   <si>
-    <t>snacks</t>
-  </si>
-  <si>
-    <t>tea,coffe</t>
+    <t>https://media.istockphoto.com/id/184567890/photo/tea-bun.jpg</t>
   </si>
   <si>
     <t>tea</t>
   </si>
   <si>
+    <t>https://images.unsplash.com/photo-1511920170033-f8396924c348?ixlib=rb-4.0.3&amp;auto=format&amp;fit=crop&amp;w=600&amp;q=80</t>
+  </si>
+  <si>
     <t>coffee</t>
   </si>
   <si>
+    <t>https://images.unsplash.com/photo-1544787219-7f47ccb76574?ixlib=rb-4.0.3&amp;auto=format&amp;fit=crop&amp;w=600&amp;q=80</t>
+  </si>
+  <si>
     <t>badam pal</t>
   </si>
   <si>
+    <t>https://images.unsplash.com/photo-1497935586351-b67a49e012bf?ixlib=rb-4.0.3&amp;auto=format&amp;fit=crop&amp;w=600&amp;q=80</t>
+  </si>
+  <si>
     <t>sukku tea</t>
   </si>
   <si>
+    <t>https://media.istockphoto.com/id/531234567/photo/badam-milk.jpg</t>
+  </si>
+  <si>
     <t>milk</t>
   </si>
   <si>
+    <t>https://media.istockphoto.com/id/642345678/photo/ginger-tea.jpg</t>
+  </si>
+  <si>
     <t>boost</t>
   </si>
   <si>
+    <t>https://images.unsplash.com/photo-1550583724-b2692b85b150?ixlib=rb-4.0.3&amp;auto=format&amp;fit=crop&amp;w=600&amp;q=80</t>
+  </si>
+  <si>
     <t>horlicks</t>
   </si>
   <si>
+    <t>https://media.istockphoto.com/id/753421987/photo/chocolate-malt-drink.jpg</t>
+  </si>
+  <si>
     <t>apple juice</t>
   </si>
   <si>
+    <t>https://media.istockphoto.com/id/864532109/photo/malted-drink.jpg</t>
+  </si>
+  <si>
     <t>orange juice</t>
   </si>
   <si>
+    <t>https://images.unsplash.com/photo-1570913149827-5296d116301f?ixlib=rb-4.0.3&amp;auto=format&amp;fit=crop&amp;w=600&amp;q=80</t>
+  </si>
+  <si>
     <t>madhulai juice</t>
   </si>
   <si>
+    <t>https://images.unsplash.com/photo-1613478223719-2ab802602423?ixlib=rb-4.0.3&amp;auto=format&amp;fit=crop&amp;w=600&amp;q=80</t>
+  </si>
+  <si>
     <t>sathukudi juice</t>
   </si>
   <si>
+    <t>https://images.unsplash.com/photo-1623065422902-30a2d299bbe4?ixlib=rb-4.0.3&amp;auto=format&amp;fit=crop&amp;w=600&amp;q=80</t>
+  </si>
+  <si>
     <t>mulampalam juice</t>
+  </si>
+  <si>
+    <t>https://media.istockphoto.com/id/975310864/photo/sweet-lime-juice.jpg</t>
+  </si>
+  <si>
+    <t>https://media.istockphoto.com/id/864209753/photo/cantaloupe-juice.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -185,11 +629,253 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -207,18 +893,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -267,7 +998,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -300,26 +1031,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -352,23 +1066,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -510,30 +1207,26 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2704779-E7DD-4171-92E2-0C849B7CDE80}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.5555555555556" customWidth="1"/>
+    <col min="4" max="4" width="160.472222222222" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" ht="16.8" customHeight="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -543,13 +1236,15 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" ht="16.8" customHeight="1" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -557,9 +1252,9 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3">
         <v>17</v>
@@ -567,12 +1262,14 @@
       <c r="C3" s="2">
         <v>5</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3">
         <v>22</v>
@@ -580,12 +1277,14 @@
       <c r="C4" s="2">
         <v>5</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" ht="18" customHeight="1" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>22</v>
@@ -593,10 +1292,12 @@
       <c r="C5" s="2">
         <v>5</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" ht="18" customHeight="1" spans="1:5">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -606,12 +1307,14 @@
       <c r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3">
         <v>20</v>
@@ -619,12 +1322,14 @@
       <c r="C7" s="2">
         <v>5</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3">
         <v>25</v>
@@ -632,12 +1337,14 @@
       <c r="C8" s="2">
         <v>5</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" ht="13.8" customHeight="1" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3">
         <v>30</v>
@@ -645,12 +1352,14 @@
       <c r="C9" s="2">
         <v>5</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" ht="13.8" customHeight="1" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3">
         <v>30</v>
@@ -658,12 +1367,14 @@
       <c r="C10" s="2">
         <v>5</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3">
         <v>25</v>
@@ -671,12 +1382,14 @@
       <c r="C11" s="2">
         <v>5</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3">
         <v>40</v>
@@ -684,12 +1397,14 @@
       <c r="C12" s="2">
         <v>5</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" t="s">
+        <v>24</v>
+      </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3">
         <v>60</v>
@@ -697,12 +1412,14 @@
       <c r="C13" s="2">
         <v>5</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" ht="18" customHeight="1" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3">
         <v>50</v>
@@ -710,12 +1427,14 @@
       <c r="C14" s="2">
         <v>5</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" ht="18" customHeight="1" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3">
         <v>15</v>
@@ -723,12 +1442,14 @@
       <c r="C15" s="2">
         <v>5</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B16" s="3">
         <v>15</v>
@@ -736,12 +1457,14 @@
       <c r="C16" s="2">
         <v>5</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B17" s="3">
         <v>15</v>
@@ -749,12 +1472,14 @@
       <c r="C17" s="2">
         <v>5</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B18" s="3">
         <v>15</v>
@@ -762,12 +1487,14 @@
       <c r="C18" s="2">
         <v>5</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B19" s="3">
         <v>15</v>
@@ -775,12 +1502,14 @@
       <c r="C19" s="2">
         <v>5</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="B20" s="3">
         <v>15</v>
@@ -788,12 +1517,14 @@
       <c r="C20" s="2">
         <v>5</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4">
       <c r="A21" s="5" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B21" s="6">
         <v>15</v>
@@ -801,10 +1532,13 @@
       <c r="C21" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="5" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="B22" s="6">
         <v>15</v>
@@ -812,10 +1546,13 @@
       <c r="C22" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="5" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="B23" s="6">
         <v>15</v>
@@ -823,10 +1560,13 @@
       <c r="C23" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="5" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="B24" s="6">
         <v>30</v>
@@ -834,10 +1574,13 @@
       <c r="C24" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="5" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B25" s="6">
         <v>8</v>
@@ -845,59 +1588,83 @@
       <c r="C25" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="B26" s="6">
+        <v>12</v>
+      </c>
+      <c r="C26" s="5">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="5" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="B27" s="6">
+        <v>15</v>
+      </c>
+      <c r="C27" s="5">
+        <v>5</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="6">
+        <v>25</v>
+      </c>
+      <c r="C28" s="5">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="6">
         <v>12</v>
       </c>
-      <c r="C27" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="6">
-        <v>15</v>
-      </c>
-      <c r="C28" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="6">
-        <v>25</v>
-      </c>
       <c r="C29" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="5" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="B30" s="6">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C30" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="5" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="B31" s="6">
         <v>20</v>
@@ -905,10 +1672,13 @@
       <c r="C31" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="5" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="B32" s="6">
         <v>20</v>
@@ -916,21 +1686,27 @@
       <c r="C32" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="5" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="B33" s="6">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C33" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="5" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="B34" s="6">
         <v>60</v>
@@ -938,10 +1714,13 @@
       <c r="C34" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="5" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="B35" s="6">
         <v>60</v>
@@ -949,10 +1728,13 @@
       <c r="C35" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="5" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B36" s="6">
         <v>60</v>
@@ -960,10 +1742,13 @@
       <c r="C36" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="5" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="B37" s="6">
         <v>60</v>
@@ -971,19 +1756,20 @@
       <c r="C37" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="6">
-        <v>60</v>
-      </c>
-      <c r="C38" s="5">
-        <v>5</v>
+      <c r="D37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4">
+      <c r="D38" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D27" r:id="rId1" display="https://images.unsplash.com/photo-1544787219-7f47ccb76574?ixlib=rb-4.0.3&amp;auto=format&amp;fit=crop&amp;w=600&amp;q=80"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>